<commit_message>
chore: update Sheets via scheduled runner
</commit_message>
<xml_diff>
--- a/Sheets/Adamantoise_Profits.xlsx
+++ b/Sheets/Adamantoise_Profits.xlsx
@@ -2604,25 +2604,25 @@
         <v>5505</v>
       </c>
       <c r="H40" t="n">
-        <v>3136.5557</v>
+        <v>3341.9583</v>
       </c>
       <c r="I40" t="n">
-        <v>2214.3845</v>
+        <v>2573.3635</v>
       </c>
       <c r="J40" t="n">
-        <v>3992.8572</v>
+        <v>3992.3076</v>
       </c>
       <c r="K40" t="n">
-        <v>2214.3845</v>
+        <v>2573.3635</v>
       </c>
       <c r="L40" t="n">
-        <v>3992.8572</v>
+        <v>3992.3076</v>
       </c>
       <c r="M40" t="n">
-        <v>-2039.3845</v>
+        <v>-2398.3635</v>
       </c>
       <c r="N40" t="n">
-        <v>-4342.8572</v>
+        <v>-4342.3076</v>
       </c>
     </row>
     <row r="41">
@@ -4440,22 +4440,19 @@
         <v>12602</v>
       </c>
       <c r="H76" t="n">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="I76" t="n">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="J76" t="n">
         <v>0</v>
       </c>
       <c r="K76" t="n">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="L76" t="n">
         <v>0</v>
-      </c>
-      <c r="M76" t="n">
-        <v>-9684</v>
       </c>
     </row>
     <row r="77">
@@ -4590,22 +4587,19 @@
         <v>12602</v>
       </c>
       <c r="H79" t="n">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
       </c>
       <c r="K79" t="n">
-        <v>9999</v>
+        <v>0</v>
       </c>
       <c r="L79" t="n">
         <v>0</v>
-      </c>
-      <c r="M79" t="n">
-        <v>-8907</v>
       </c>
     </row>
     <row r="80">
@@ -4639,25 +4633,25 @@
         <v>12605</v>
       </c>
       <c r="H80" t="n">
-        <v>109108900</v>
+        <v>100016910</v>
       </c>
       <c r="I80" t="n">
         <v>166678160</v>
       </c>
       <c r="J80" t="n">
-        <v>40025772</v>
+        <v>33355662</v>
       </c>
       <c r="K80" t="n">
         <v>500034480</v>
       </c>
       <c r="L80" t="n">
-        <v>120077316</v>
+        <v>100066986</v>
       </c>
       <c r="M80" t="n">
         <v>-500033482</v>
       </c>
       <c r="N80" t="n">
-        <v>-120079312</v>
+        <v>-100068982</v>
       </c>
     </row>
     <row r="81">
@@ -4786,25 +4780,25 @@
         <v>12605</v>
       </c>
       <c r="H83" t="n">
-        <v>109108900</v>
+        <v>100016910</v>
       </c>
       <c r="I83" t="n">
         <v>166678160</v>
       </c>
       <c r="J83" t="n">
-        <v>40025772</v>
+        <v>33355662</v>
       </c>
       <c r="K83" t="n">
         <v>1500103440</v>
       </c>
       <c r="L83" t="n">
-        <v>360231948</v>
+        <v>300200958</v>
       </c>
       <c r="M83" t="n">
         <v>-1500098448</v>
       </c>
       <c r="N83" t="n">
-        <v>-360241932</v>
+        <v>-300210942</v>
       </c>
     </row>
     <row r="84">
@@ -5530,22 +5524,22 @@
         <v>36237</v>
       </c>
       <c r="H98" t="n">
-        <v>2116.1082</v>
+        <v>2117.1353</v>
       </c>
       <c r="I98" t="n">
-        <v>1832.2941</v>
+        <v>1833.4117</v>
       </c>
       <c r="J98" t="n">
         <v>5332.6665</v>
       </c>
       <c r="K98" t="n">
-        <v>1832.2941</v>
+        <v>1833.4117</v>
       </c>
       <c r="L98" t="n">
         <v>5332.6665</v>
       </c>
       <c r="M98" t="n">
-        <v>-334.2941000000001</v>
+        <v>-335.4117000000001</v>
       </c>
       <c r="N98" t="n">
         <v>-8328.666499999999</v>
@@ -6292,22 +6286,19 @@
         <v>27775</v>
       </c>
       <c r="H113" t="n">
-        <v>1255</v>
+        <v>0</v>
       </c>
       <c r="I113" t="n">
-        <v>1255</v>
+        <v>0</v>
       </c>
       <c r="J113" t="n">
         <v>0</v>
       </c>
       <c r="K113" t="n">
-        <v>1255</v>
+        <v>0</v>
       </c>
       <c r="L113" t="n">
         <v>0</v>
-      </c>
-      <c r="M113" t="n">
-        <v>1999</v>
       </c>
     </row>
     <row r="114">
@@ -6742,22 +6733,22 @@
         <v>36237</v>
       </c>
       <c r="H122" t="n">
-        <v>2116.1082</v>
+        <v>2117.1353</v>
       </c>
       <c r="I122" t="n">
-        <v>1832.2941</v>
+        <v>1833.4117</v>
       </c>
       <c r="J122" t="n">
         <v>5332.6665</v>
       </c>
       <c r="K122" t="n">
-        <v>5496.8823</v>
+        <v>5500.2351</v>
       </c>
       <c r="L122" t="n">
         <v>15997.9995</v>
       </c>
       <c r="M122" t="n">
-        <v>-3046.8823</v>
+        <v>-3050.2351</v>
       </c>
       <c r="N122" t="n">
         <v>-20897.9995</v>
@@ -6938,22 +6929,22 @@
         <v>34391</v>
       </c>
       <c r="H126" t="n">
-        <v>88499.75</v>
+        <v>174000</v>
       </c>
       <c r="I126" t="n">
         <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>88499.75</v>
+        <v>174000</v>
       </c>
       <c r="K126" t="n">
         <v>0</v>
       </c>
       <c r="L126" t="n">
-        <v>88499.75</v>
+        <v>174000</v>
       </c>
       <c r="N126" t="n">
-        <v>-98379.75</v>
+        <v>-183880</v>
       </c>
     </row>
     <row r="127">
@@ -7241,22 +7232,22 @@
         <v>44049</v>
       </c>
       <c r="H132" t="n">
-        <v>4089.4</v>
+        <v>3998.561</v>
       </c>
       <c r="I132" t="n">
-        <v>4102.3516</v>
+        <v>4004</v>
       </c>
       <c r="J132" t="n">
         <v>3929.6667</v>
       </c>
       <c r="K132" t="n">
-        <v>12307.0548</v>
+        <v>12012</v>
       </c>
       <c r="L132" t="n">
         <v>11789.0001</v>
       </c>
       <c r="M132" t="n">
-        <v>-9777.0548</v>
+        <v>-9482</v>
       </c>
       <c r="N132" t="n">
         <v>-16849.0001</v>
@@ -7486,22 +7477,22 @@
         <v>44013</v>
       </c>
       <c r="H137" t="n">
-        <v>38227.543</v>
+        <v>36770.4</v>
       </c>
       <c r="I137" t="n">
-        <v>66573.92</v>
+        <v>61947.145</v>
       </c>
       <c r="J137" t="n">
         <v>4727.273</v>
       </c>
       <c r="K137" t="n">
-        <v>199721.76</v>
+        <v>185841.435</v>
       </c>
       <c r="L137" t="n">
         <v>14181.819</v>
       </c>
       <c r="M137" t="n">
-        <v>-197171.76</v>
+        <v>-183291.435</v>
       </c>
       <c r="N137" t="n">
         <v>-19281.819</v>
@@ -7538,25 +7529,25 @@
         <v>44169</v>
       </c>
       <c r="H138" t="n">
-        <v>8312.339</v>
+        <v>8065.1665</v>
       </c>
       <c r="I138" t="n">
-        <v>7799.3335</v>
+        <v>6338.6</v>
       </c>
       <c r="J138" t="n">
-        <v>8338.424000000001</v>
+        <v>8206.688</v>
       </c>
       <c r="K138" t="n">
-        <v>23398.0005</v>
+        <v>19015.8</v>
       </c>
       <c r="L138" t="n">
-        <v>25015.272</v>
+        <v>24620.064</v>
       </c>
       <c r="M138" t="n">
-        <v>-18258.0005</v>
+        <v>-13875.8</v>
       </c>
       <c r="N138" t="n">
-        <v>-35295.272</v>
+        <v>-34900.064</v>
       </c>
     </row>
     <row r="139">
@@ -8226,22 +8217,22 @@
         <v>2662</v>
       </c>
       <c r="H10" t="n">
-        <v>4457029.5</v>
+        <v>5730280.5</v>
       </c>
       <c r="I10" t="n">
-        <v>13333767</v>
+        <v>40000000</v>
       </c>
       <c r="J10" t="n">
         <v>18660.666</v>
       </c>
       <c r="K10" t="n">
-        <v>13333767</v>
+        <v>40000000</v>
       </c>
       <c r="L10" t="n">
         <v>18660.666</v>
       </c>
       <c r="M10" t="n">
-        <v>-13333597</v>
+        <v>-39999830</v>
       </c>
       <c r="N10" t="n">
         <v>-19000.666</v>
@@ -8379,25 +8370,25 @@
         <v>2656</v>
       </c>
       <c r="H13" t="n">
-        <v>657.1429000000001</v>
+        <v>437.33334</v>
       </c>
       <c r="I13" t="n">
         <v>100</v>
       </c>
       <c r="J13" t="n">
-        <v>750</v>
+        <v>504.8</v>
       </c>
       <c r="K13" t="n">
         <v>100</v>
       </c>
       <c r="L13" t="n">
-        <v>750</v>
+        <v>504.8</v>
       </c>
       <c r="M13" t="n">
         <v>44</v>
       </c>
       <c r="N13" t="n">
-        <v>-1038</v>
+        <v>-792.8</v>
       </c>
     </row>
     <row r="14">
@@ -8431,25 +8422,25 @@
         <v>2673</v>
       </c>
       <c r="H14" t="n">
-        <v>424.75</v>
+        <v>8355.286</v>
       </c>
       <c r="I14" t="n">
-        <v>100</v>
+        <v>490</v>
       </c>
       <c r="J14" t="n">
-        <v>533</v>
+        <v>11501.4</v>
       </c>
       <c r="K14" t="n">
-        <v>100</v>
+        <v>490</v>
       </c>
       <c r="L14" t="n">
-        <v>533</v>
+        <v>11501.4</v>
       </c>
       <c r="M14" t="n">
-        <v>75</v>
+        <v>-315</v>
       </c>
       <c r="N14" t="n">
-        <v>-883</v>
+        <v>-11851.4</v>
       </c>
     </row>
     <row r="15">
@@ -9028,25 +9019,25 @@
         <v>2241</v>
       </c>
       <c r="H26" t="n">
-        <v>15266.667</v>
+        <v>15200</v>
       </c>
       <c r="I26" t="n">
         <v>300</v>
       </c>
       <c r="J26" t="n">
-        <v>22750</v>
+        <v>45000</v>
       </c>
       <c r="K26" t="n">
         <v>300</v>
       </c>
       <c r="L26" t="n">
-        <v>22750</v>
+        <v>45000</v>
       </c>
       <c r="M26" t="n">
         <v>30</v>
       </c>
       <c r="N26" t="n">
-        <v>-23410</v>
+        <v>-45660</v>
       </c>
     </row>
     <row r="27">
@@ -9178,22 +9169,22 @@
         <v>3557</v>
       </c>
       <c r="H29" t="n">
-        <v>7505</v>
+        <v>15000</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>7505</v>
+        <v>15000</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>7505</v>
+        <v>15000</v>
       </c>
       <c r="N29" t="n">
-        <v>-8121</v>
+        <v>-15616</v>
       </c>
     </row>
     <row r="30">
@@ -9331,22 +9322,22 @@
         <v>44147</v>
       </c>
       <c r="H32" t="n">
-        <v>18969.121</v>
+        <v>17794.412</v>
       </c>
       <c r="I32" t="n">
-        <v>18443.375</v>
+        <v>17300.979</v>
       </c>
       <c r="J32" t="n">
         <v>39999</v>
       </c>
       <c r="K32" t="n">
-        <v>18443.375</v>
+        <v>17300.979</v>
       </c>
       <c r="L32" t="n">
         <v>39999</v>
       </c>
       <c r="M32" t="n">
-        <v>-18156.375</v>
+        <v>-17013.979</v>
       </c>
       <c r="N32" t="n">
         <v>-40573</v>
@@ -9527,22 +9518,22 @@
         <v>3068</v>
       </c>
       <c r="H36" t="n">
-        <v>2481.9</v>
+        <v>2480.5</v>
       </c>
       <c r="I36" t="n">
-        <v>2481.9</v>
+        <v>2480.5</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>2481.9</v>
+        <v>2480.5</v>
       </c>
       <c r="L36" t="n">
         <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>-2135.9</v>
+        <v>-2134.5</v>
       </c>
     </row>
     <row r="37">
@@ -9974,22 +9965,22 @@
         <v>27714</v>
       </c>
       <c r="H45" t="n">
-        <v>4023.3572</v>
+        <v>3851.9</v>
       </c>
       <c r="I45" t="n">
-        <v>4327.25</v>
+        <v>4264.875</v>
       </c>
       <c r="J45" t="n">
         <v>2200</v>
       </c>
       <c r="K45" t="n">
-        <v>4327.25</v>
+        <v>4264.875</v>
       </c>
       <c r="L45" t="n">
         <v>2200</v>
       </c>
       <c r="M45" t="n">
-        <v>-3950.25</v>
+        <v>-3887.875</v>
       </c>
       <c r="N45" t="n">
         <v>-2954</v>
@@ -11380,25 +11371,25 @@
         <v>44000</v>
       </c>
       <c r="H74" t="n">
-        <v>2499.4255</v>
+        <v>2606.0222</v>
       </c>
       <c r="I74" t="n">
-        <v>1587.4762</v>
+        <v>1635.2051</v>
       </c>
       <c r="J74" t="n">
-        <v>10159.8</v>
+        <v>8916.333000000001</v>
       </c>
       <c r="K74" t="n">
-        <v>1587.4762</v>
+        <v>1635.2051</v>
       </c>
       <c r="L74" t="n">
-        <v>10159.8</v>
+        <v>8916.333000000001</v>
       </c>
       <c r="M74" t="n">
-        <v>-713.4762000000001</v>
+        <v>-761.2050999999999</v>
       </c>
       <c r="N74" t="n">
-        <v>-11907.8</v>
+        <v>-10664.333</v>
       </c>
     </row>
     <row r="75">
@@ -11530,25 +11521,25 @@
         <v>44000</v>
       </c>
       <c r="H77" t="n">
-        <v>2499.4255</v>
+        <v>2606.0222</v>
       </c>
       <c r="I77" t="n">
-        <v>1587.4762</v>
+        <v>1635.2051</v>
       </c>
       <c r="J77" t="n">
-        <v>10159.8</v>
+        <v>8916.333000000001</v>
       </c>
       <c r="K77" t="n">
-        <v>7937.381</v>
+        <v>8176.0255</v>
       </c>
       <c r="L77" t="n">
-        <v>50799</v>
+        <v>44581.665</v>
       </c>
       <c r="M77" t="n">
-        <v>-3569.381</v>
+        <v>-3808.0255</v>
       </c>
       <c r="N77" t="n">
-        <v>-59535</v>
+        <v>-53317.665</v>
       </c>
     </row>
     <row r="78">
@@ -13138,22 +13129,22 @@
         <v>27708</v>
       </c>
       <c r="H110" t="n">
-        <v>1205.3334</v>
+        <v>1092.8823</v>
       </c>
       <c r="I110" t="n">
-        <v>1205.3334</v>
+        <v>1092.8823</v>
       </c>
       <c r="J110" t="n">
         <v>0</v>
       </c>
       <c r="K110" t="n">
-        <v>1205.3334</v>
+        <v>1092.8823</v>
       </c>
       <c r="L110" t="n">
         <v>0</v>
       </c>
       <c r="M110" t="n">
-        <v>839.6666</v>
+        <v>952.1177</v>
       </c>
     </row>
     <row r="111">
@@ -13236,22 +13227,22 @@
         <v>25808</v>
       </c>
       <c r="H112" t="n">
-        <v>55499.75</v>
+        <v>49399.6</v>
       </c>
       <c r="I112" t="n">
         <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>55499.75</v>
+        <v>49399.6</v>
       </c>
       <c r="K112" t="n">
         <v>0</v>
       </c>
       <c r="L112" t="n">
-        <v>55499.75</v>
+        <v>49399.6</v>
       </c>
       <c r="N112" t="n">
-        <v>-58453.75</v>
+        <v>-52353.6</v>
       </c>
     </row>
     <row r="113">
@@ -13334,22 +13325,22 @@
         <v>25968</v>
       </c>
       <c r="H114" t="n">
-        <v>49792.2</v>
+        <v>47658.5</v>
       </c>
       <c r="I114" t="n">
         <v>0</v>
       </c>
       <c r="J114" t="n">
-        <v>49792.2</v>
+        <v>47658.5</v>
       </c>
       <c r="K114" t="n">
         <v>0</v>
       </c>
       <c r="L114" t="n">
-        <v>49792.2</v>
+        <v>47658.5</v>
       </c>
       <c r="N114" t="n">
-        <v>-58470.2</v>
+        <v>-56336.5</v>
       </c>
     </row>
     <row r="115">
@@ -13726,22 +13717,22 @@
         <v>36168</v>
       </c>
       <c r="H122" t="n">
-        <v>6471.8667</v>
+        <v>6593.9136</v>
       </c>
       <c r="I122" t="n">
-        <v>5955.5684</v>
+        <v>6099.524</v>
       </c>
       <c r="J122" t="n">
         <v>7891.6875</v>
       </c>
       <c r="K122" t="n">
-        <v>17866.7052</v>
+        <v>18298.572</v>
       </c>
       <c r="L122" t="n">
         <v>23675.0625</v>
       </c>
       <c r="M122" t="n">
-        <v>-15416.7052</v>
+        <v>-15848.572</v>
       </c>
       <c r="N122" t="n">
         <v>-28575.0625</v>
@@ -13876,22 +13867,22 @@
         <v>34251</v>
       </c>
       <c r="H125" t="n">
-        <v>126244.75</v>
+        <v>124994.75</v>
       </c>
       <c r="I125" t="n">
         <v>0</v>
       </c>
       <c r="J125" t="n">
-        <v>126244.75</v>
+        <v>124994.75</v>
       </c>
       <c r="K125" t="n">
         <v>0</v>
       </c>
       <c r="L125" t="n">
-        <v>126244.75</v>
+        <v>124994.75</v>
       </c>
       <c r="N125" t="n">
-        <v>-136084.75</v>
+        <v>-134834.75</v>
       </c>
     </row>
     <row r="126">
@@ -14219,22 +14210,22 @@
         <v>43997</v>
       </c>
       <c r="H132" t="n">
-        <v>420036.28</v>
+        <v>373521.6</v>
       </c>
       <c r="I132" t="n">
-        <v>627554.75</v>
+        <v>528688.8</v>
       </c>
       <c r="J132" t="n">
         <v>4999.375</v>
       </c>
       <c r="K132" t="n">
-        <v>1882664.25</v>
+        <v>1586066.4</v>
       </c>
       <c r="L132" t="n">
         <v>14998.125</v>
       </c>
       <c r="M132" t="n">
-        <v>-1880134.25</v>
+        <v>-1583536.4</v>
       </c>
       <c r="N132" t="n">
         <v>-20058.125</v>
@@ -15691,22 +15682,22 @@
         <v>14149</v>
       </c>
       <c r="H20" t="n">
-        <v>21737.75</v>
+        <v>20907.24</v>
       </c>
       <c r="I20" t="n">
-        <v>34776.285</v>
+        <v>32522.867</v>
       </c>
       <c r="J20" t="n">
         <v>3483.8</v>
       </c>
       <c r="K20" t="n">
-        <v>34776.285</v>
+        <v>32522.867</v>
       </c>
       <c r="L20" t="n">
         <v>3483.8</v>
       </c>
       <c r="M20" t="n">
-        <v>-34529.285</v>
+        <v>-32275.867</v>
       </c>
       <c r="N20" t="n">
         <v>-3977.8</v>
@@ -16190,26 +16181,23 @@
         <v>1609</v>
       </c>
       <c r="H30" t="n">
-        <v>1276.6666</v>
+        <v>409.5</v>
       </c>
       <c r="I30" t="n">
         <v>409.5</v>
       </c>
       <c r="J30" t="n">
-        <v>3011</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
         <v>409.5</v>
       </c>
       <c r="L30" t="n">
-        <v>3011</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
         <v>-284.5</v>
       </c>
-      <c r="N30" t="n">
-        <v>-3261</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -17596,22 +17584,19 @@
         <v>43223</v>
       </c>
       <c r="H59" t="n">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
       </c>
       <c r="J59" t="n">
-        <v>120000</v>
+        <v>0</v>
       </c>
       <c r="K59" t="n">
         <v>0</v>
       </c>
       <c r="L59" t="n">
-        <v>120000</v>
-      </c>
-      <c r="N59" t="n">
-        <v>-121694</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -18625,25 +18610,25 @@
         <v>13747</v>
       </c>
       <c r="H80" t="n">
-        <v>783.2632</v>
+        <v>779.1875</v>
       </c>
       <c r="I80" t="n">
-        <v>521.1429000000001</v>
+        <v>524.6667</v>
       </c>
       <c r="J80" t="n">
-        <v>936.1667</v>
+        <v>931.9</v>
       </c>
       <c r="K80" t="n">
-        <v>521.1429000000001</v>
+        <v>524.6667</v>
       </c>
       <c r="L80" t="n">
-        <v>936.1667</v>
+        <v>931.9</v>
       </c>
       <c r="M80" t="n">
-        <v>476.8570999999999</v>
+        <v>473.3333</v>
       </c>
       <c r="N80" t="n">
-        <v>-2932.1667</v>
+        <v>-2927.9</v>
       </c>
     </row>
     <row r="81">
@@ -18778,25 +18763,25 @@
         <v>13747</v>
       </c>
       <c r="H83" t="n">
-        <v>783.2632</v>
+        <v>779.1875</v>
       </c>
       <c r="I83" t="n">
-        <v>521.1429000000001</v>
+        <v>524.6667</v>
       </c>
       <c r="J83" t="n">
-        <v>936.1667</v>
+        <v>931.9</v>
       </c>
       <c r="K83" t="n">
-        <v>2605.7145</v>
+        <v>2623.3335</v>
       </c>
       <c r="L83" t="n">
-        <v>4680.8335</v>
+        <v>4659.5</v>
       </c>
       <c r="M83" t="n">
-        <v>2386.2855</v>
+        <v>2368.6665</v>
       </c>
       <c r="N83" t="n">
-        <v>-14664.8335</v>
+        <v>-14643.5</v>
       </c>
     </row>
     <row r="84">
@@ -18931,25 +18916,25 @@
         <v>12526</v>
       </c>
       <c r="H86" t="n">
-        <v>4890.75</v>
+        <v>4848.5</v>
       </c>
       <c r="I86" t="n">
-        <v>4089.6</v>
+        <v>3853.2727</v>
       </c>
       <c r="J86" t="n">
-        <v>8896.5</v>
+        <v>8497.666999999999</v>
       </c>
       <c r="K86" t="n">
-        <v>4089.6</v>
+        <v>3853.2727</v>
       </c>
       <c r="L86" t="n">
-        <v>8896.5</v>
+        <v>8497.666999999999</v>
       </c>
       <c r="M86" t="n">
-        <v>-2966.6</v>
+        <v>-2730.2727</v>
       </c>
       <c r="N86" t="n">
-        <v>-11142.5</v>
+        <v>-10743.667</v>
       </c>
     </row>
     <row r="87">
@@ -19081,25 +19066,25 @@
         <v>12526</v>
       </c>
       <c r="H89" t="n">
-        <v>4890.75</v>
+        <v>4848.5</v>
       </c>
       <c r="I89" t="n">
-        <v>4089.6</v>
+        <v>3853.2727</v>
       </c>
       <c r="J89" t="n">
-        <v>8896.5</v>
+        <v>8497.666999999999</v>
       </c>
       <c r="K89" t="n">
-        <v>20448</v>
+        <v>19266.3635</v>
       </c>
       <c r="L89" t="n">
-        <v>44482.5</v>
+        <v>42488.335</v>
       </c>
       <c r="M89" t="n">
-        <v>-14832</v>
+        <v>-13650.3635</v>
       </c>
       <c r="N89" t="n">
-        <v>-55714.5</v>
+        <v>-53720.335</v>
       </c>
     </row>
     <row r="90">
@@ -19329,22 +19314,22 @@
         <v>19939</v>
       </c>
       <c r="H94" t="n">
-        <v>1715.4082</v>
+        <v>1682.02</v>
       </c>
       <c r="I94" t="n">
-        <v>1659.909</v>
+        <v>1624.0444</v>
       </c>
       <c r="J94" t="n">
         <v>2203.8</v>
       </c>
       <c r="K94" t="n">
-        <v>1659.909</v>
+        <v>1624.0444</v>
       </c>
       <c r="L94" t="n">
         <v>2203.8</v>
       </c>
       <c r="M94" t="n">
-        <v>-1208.909</v>
+        <v>-1173.0444</v>
       </c>
       <c r="N94" t="n">
         <v>-3105.8</v>
@@ -19880,22 +19865,22 @@
         <v>19947</v>
       </c>
       <c r="H105" t="n">
-        <v>2054.182</v>
+        <v>1947.6666</v>
       </c>
       <c r="I105" t="n">
-        <v>1261.0588</v>
+        <v>1210</v>
       </c>
       <c r="J105" t="n">
         <v>4750.8</v>
       </c>
       <c r="K105" t="n">
-        <v>1261.0588</v>
+        <v>1210</v>
       </c>
       <c r="L105" t="n">
         <v>4750.8</v>
       </c>
       <c r="M105" t="n">
-        <v>485.9412</v>
+        <v>537</v>
       </c>
       <c r="N105" t="n">
         <v>-8244.799999999999</v>
@@ -19981,19 +19966,25 @@
         <v>27706</v>
       </c>
       <c r="H107" t="n">
-        <v>0</v>
+        <v>3998.75</v>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>3995</v>
       </c>
       <c r="J107" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="K107" t="n">
-        <v>0</v>
+        <v>3995</v>
       </c>
       <c r="L107" t="n">
-        <v>0</v>
+        <v>4000</v>
+      </c>
+      <c r="M107" t="n">
+        <v>-2075</v>
+      </c>
+      <c r="N107" t="n">
+        <v>-7840</v>
       </c>
     </row>
     <row r="108">
@@ -21301,25 +21292,25 @@
         <v>43998</v>
       </c>
       <c r="H134" t="n">
-        <v>6730</v>
+        <v>5720.5</v>
       </c>
       <c r="I134" t="n">
-        <v>4518.3335</v>
+        <v>4150.625</v>
       </c>
       <c r="J134" t="n">
-        <v>20000</v>
+        <v>12000</v>
       </c>
       <c r="K134" t="n">
-        <v>13555.0005</v>
+        <v>12451.875</v>
       </c>
       <c r="L134" t="n">
-        <v>60000</v>
+        <v>36000</v>
       </c>
       <c r="M134" t="n">
-        <v>-11020.0005</v>
+        <v>-9916.875</v>
       </c>
       <c r="N134" t="n">
-        <v>-65070</v>
+        <v>-41070</v>
       </c>
     </row>
     <row r="135">
@@ -23238,25 +23229,25 @@
         <v>44023</v>
       </c>
       <c r="H31" t="n">
-        <v>7492.8</v>
+        <v>7306.9653</v>
       </c>
       <c r="I31" t="n">
-        <v>3754.2368</v>
+        <v>3709.2307</v>
       </c>
       <c r="J31" t="n">
-        <v>15849.588</v>
+        <v>14691.789</v>
       </c>
       <c r="K31" t="n">
-        <v>3754.2368</v>
+        <v>3709.2307</v>
       </c>
       <c r="L31" t="n">
-        <v>15849.588</v>
+        <v>14691.789</v>
       </c>
       <c r="M31" t="n">
-        <v>-3459.2368</v>
+        <v>-3414.2307</v>
       </c>
       <c r="N31" t="n">
-        <v>-16439.588</v>
+        <v>-15281.789</v>
       </c>
     </row>
     <row r="32">
@@ -23391,25 +23382,25 @@
         <v>44023</v>
       </c>
       <c r="H34" t="n">
-        <v>7492.8</v>
+        <v>7306.9653</v>
       </c>
       <c r="I34" t="n">
-        <v>3754.2368</v>
+        <v>3709.2307</v>
       </c>
       <c r="J34" t="n">
-        <v>15849.588</v>
+        <v>14691.789</v>
       </c>
       <c r="K34" t="n">
-        <v>3754.2368</v>
+        <v>3709.2307</v>
       </c>
       <c r="L34" t="n">
-        <v>15849.588</v>
+        <v>14691.789</v>
       </c>
       <c r="M34" t="n">
-        <v>-3552.2368</v>
+        <v>-3507.2307</v>
       </c>
       <c r="N34" t="n">
-        <v>-16253.588</v>
+        <v>-15095.789</v>
       </c>
     </row>
     <row r="35">
@@ -24570,25 +24561,25 @@
         <v>44021</v>
       </c>
       <c r="H58" t="n">
-        <v>4342.6523</v>
+        <v>4917</v>
       </c>
       <c r="I58" t="n">
-        <v>1992.5625</v>
+        <v>2237.7693</v>
       </c>
       <c r="J58" t="n">
-        <v>9714.286</v>
+        <v>8400</v>
       </c>
       <c r="K58" t="n">
-        <v>1992.5625</v>
+        <v>2237.7693</v>
       </c>
       <c r="L58" t="n">
-        <v>9714.286</v>
+        <v>8400</v>
       </c>
       <c r="M58" t="n">
-        <v>-1789.5625</v>
+        <v>-2034.7693</v>
       </c>
       <c r="N58" t="n">
-        <v>-10120.286</v>
+        <v>-8806</v>
       </c>
     </row>
     <row r="59">
@@ -26870,25 +26861,25 @@
         <v>19928</v>
       </c>
       <c r="H105" t="n">
-        <v>994.375</v>
+        <v>858.7273</v>
       </c>
       <c r="I105" t="n">
-        <v>990.8</v>
+        <v>816.1111</v>
       </c>
       <c r="J105" t="n">
-        <v>1000.3333</v>
+        <v>1050.5</v>
       </c>
       <c r="K105" t="n">
-        <v>990.8</v>
+        <v>816.1111</v>
       </c>
       <c r="L105" t="n">
-        <v>1000.3333</v>
+        <v>1050.5</v>
       </c>
       <c r="M105" t="n">
-        <v>756.2</v>
+        <v>930.8889</v>
       </c>
       <c r="N105" t="n">
-        <v>-4494.3333</v>
+        <v>-4544.5</v>
       </c>
     </row>
     <row r="106">
@@ -27712,25 +27703,25 @@
         <v>36196</v>
       </c>
       <c r="H122" t="n">
-        <v>20008640</v>
+        <v>16674033</v>
       </c>
       <c r="I122" t="n">
         <v>25001050</v>
       </c>
       <c r="J122" t="n">
-        <v>39000</v>
+        <v>20000</v>
       </c>
       <c r="K122" t="n">
         <v>75003150</v>
       </c>
       <c r="L122" t="n">
-        <v>117000</v>
+        <v>60000</v>
       </c>
       <c r="M122" t="n">
         <v>-75000700</v>
       </c>
       <c r="N122" t="n">
-        <v>-121900</v>
+        <v>-64900</v>
       </c>
     </row>
     <row r="123">
@@ -28205,22 +28196,22 @@
         <v>44019</v>
       </c>
       <c r="H132" t="n">
-        <v>3238.6365</v>
+        <v>2985.5625</v>
       </c>
       <c r="I132" t="n">
-        <v>2758.3333</v>
+        <v>2640.6428</v>
       </c>
       <c r="J132" t="n">
         <v>5400</v>
       </c>
       <c r="K132" t="n">
-        <v>8274.999899999999</v>
+        <v>7921.928400000001</v>
       </c>
       <c r="L132" t="n">
         <v>16200</v>
       </c>
       <c r="M132" t="n">
-        <v>-5744.999899999999</v>
+        <v>-5391.928400000001</v>
       </c>
       <c r="N132" t="n">
         <v>-21260</v>
@@ -28404,25 +28395,25 @@
         <v>44021</v>
       </c>
       <c r="H136" t="n">
-        <v>4342.6523</v>
+        <v>4917</v>
       </c>
       <c r="I136" t="n">
-        <v>1992.5625</v>
+        <v>2237.7693</v>
       </c>
       <c r="J136" t="n">
-        <v>9714.286</v>
+        <v>8400</v>
       </c>
       <c r="K136" t="n">
-        <v>5977.6875</v>
+        <v>6713.3079</v>
       </c>
       <c r="L136" t="n">
-        <v>29142.858</v>
+        <v>25200</v>
       </c>
       <c r="M136" t="n">
-        <v>-3427.6875</v>
+        <v>-4163.3079</v>
       </c>
       <c r="N136" t="n">
-        <v>-34242.858</v>
+        <v>-30300</v>
       </c>
     </row>
     <row r="137">
@@ -28649,25 +28640,25 @@
         <v>43345</v>
       </c>
       <c r="H141" t="n">
-        <v>586680.4399999999</v>
+        <v>540713.2</v>
       </c>
       <c r="I141" t="n">
         <v>49500</v>
       </c>
       <c r="J141" t="n">
-        <v>658304.4399999999</v>
+        <v>598502.9399999999</v>
       </c>
       <c r="K141" t="n">
         <v>49500</v>
       </c>
       <c r="L141" t="n">
-        <v>658304.4399999999</v>
+        <v>598502.9399999999</v>
       </c>
       <c r="M141" t="n">
         <v>-44320</v>
       </c>
       <c r="N141" t="n">
-        <v>-668664.4399999999</v>
+        <v>-608862.9399999999</v>
       </c>
     </row>
   </sheetData>
@@ -33022,22 +33013,22 @@
         <v>12892</v>
       </c>
       <c r="H86" t="n">
-        <v>1449.75</v>
+        <v>2500</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
       </c>
       <c r="J86" t="n">
-        <v>1449.75</v>
+        <v>2500</v>
       </c>
       <c r="K86" t="n">
         <v>0</v>
       </c>
       <c r="L86" t="n">
-        <v>4349.25</v>
+        <v>7500</v>
       </c>
       <c r="N86" t="n">
-        <v>-6721.25</v>
+        <v>-9872</v>
       </c>
     </row>
     <row r="87">
@@ -33166,22 +33157,22 @@
         <v>12892</v>
       </c>
       <c r="H89" t="n">
-        <v>1449.75</v>
+        <v>2500</v>
       </c>
       <c r="I89" t="n">
         <v>0</v>
       </c>
       <c r="J89" t="n">
-        <v>1449.75</v>
+        <v>2500</v>
       </c>
       <c r="K89" t="n">
         <v>0</v>
       </c>
       <c r="L89" t="n">
-        <v>13047.75</v>
+        <v>22500</v>
       </c>
       <c r="N89" t="n">
-        <v>-24903.75</v>
+        <v>-34356</v>
       </c>
     </row>
     <row r="90">
@@ -34054,25 +34045,25 @@
         <v>27838</v>
       </c>
       <c r="H107" t="n">
-        <v>1165</v>
+        <v>1019.1071</v>
       </c>
       <c r="I107" t="n">
-        <v>632.7778</v>
+        <v>584.5</v>
       </c>
       <c r="J107" t="n">
-        <v>1431.1111</v>
+        <v>1260.5555</v>
       </c>
       <c r="K107" t="n">
-        <v>1898.3334</v>
+        <v>1753.5</v>
       </c>
       <c r="L107" t="n">
-        <v>4293.3333</v>
+        <v>3781.6665</v>
       </c>
       <c r="M107" t="n">
-        <v>21.66660000000002</v>
+        <v>166.5</v>
       </c>
       <c r="N107" t="n">
-        <v>-8133.3333</v>
+        <v>-7621.666499999999</v>
       </c>
     </row>
     <row r="108">
@@ -39216,25 +39207,25 @@
         <v>14146</v>
       </c>
       <c r="H70" t="n">
-        <v>4514.1924</v>
+        <v>4206</v>
       </c>
       <c r="I70" t="n">
-        <v>4541</v>
+        <v>4106.8</v>
       </c>
       <c r="J70" t="n">
-        <v>4500</v>
+        <v>4261.1113</v>
       </c>
       <c r="K70" t="n">
-        <v>4541</v>
+        <v>4106.8</v>
       </c>
       <c r="L70" t="n">
-        <v>4500</v>
+        <v>4261.1113</v>
       </c>
       <c r="M70" t="n">
-        <v>-4271</v>
+        <v>-3836.8</v>
       </c>
       <c r="N70" t="n">
-        <v>-5040</v>
+        <v>-4801.1113</v>
       </c>
     </row>
     <row r="71">
@@ -39366,25 +39357,25 @@
         <v>14146</v>
       </c>
       <c r="H73" t="n">
-        <v>4514.1924</v>
+        <v>4206</v>
       </c>
       <c r="I73" t="n">
-        <v>4541</v>
+        <v>4106.8</v>
       </c>
       <c r="J73" t="n">
-        <v>4500</v>
+        <v>4261.1113</v>
       </c>
       <c r="K73" t="n">
-        <v>4541</v>
+        <v>4106.8</v>
       </c>
       <c r="L73" t="n">
-        <v>4500</v>
+        <v>4261.1113</v>
       </c>
       <c r="M73" t="n">
-        <v>-3605</v>
+        <v>-3170.8</v>
       </c>
       <c r="N73" t="n">
-        <v>-6372</v>
+        <v>-6133.1113</v>
       </c>
     </row>
     <row r="74">
@@ -39712,22 +39703,19 @@
         <v>12521</v>
       </c>
       <c r="H80" t="n">
-        <v>2503</v>
+        <v>0</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="n">
-        <v>2503</v>
+        <v>0</v>
       </c>
       <c r="K80" t="n">
         <v>0</v>
       </c>
       <c r="L80" t="n">
-        <v>2503</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-4499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -39859,22 +39847,19 @@
         <v>12521</v>
       </c>
       <c r="H83" t="n">
-        <v>2503</v>
+        <v>0</v>
       </c>
       <c r="I83" t="n">
         <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>2503</v>
+        <v>0</v>
       </c>
       <c r="K83" t="n">
         <v>0</v>
       </c>
       <c r="L83" t="n">
-        <v>12515</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-22499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -40527,25 +40512,25 @@
         <v>19940</v>
       </c>
       <c r="H97" t="n">
-        <v>1353.0625</v>
+        <v>1401.7667</v>
       </c>
       <c r="I97" t="n">
-        <v>1238.4736</v>
+        <v>1177.619</v>
       </c>
       <c r="J97" t="n">
-        <v>1520.5385</v>
+        <v>1924.7778</v>
       </c>
       <c r="K97" t="n">
-        <v>1238.4736</v>
+        <v>1177.619</v>
       </c>
       <c r="L97" t="n">
-        <v>1520.5385</v>
+        <v>1924.7778</v>
       </c>
       <c r="M97" t="n">
-        <v>-742.4736</v>
+        <v>-681.6189999999999</v>
       </c>
       <c r="N97" t="n">
-        <v>-2512.5385</v>
+        <v>-2916.7778</v>
       </c>
     </row>
     <row r="98">
@@ -40778,22 +40763,22 @@
         <v>36169</v>
       </c>
       <c r="H102" t="n">
-        <v>2363.3462</v>
+        <v>2210.2415</v>
       </c>
       <c r="I102" t="n">
-        <v>2169.182</v>
+        <v>2014.88</v>
       </c>
       <c r="J102" t="n">
         <v>3431.25</v>
       </c>
       <c r="K102" t="n">
-        <v>2169.182</v>
+        <v>2014.88</v>
       </c>
       <c r="L102" t="n">
         <v>3431.25</v>
       </c>
       <c r="M102" t="n">
-        <v>-547.1819999999998</v>
+        <v>-392.8800000000001</v>
       </c>
       <c r="N102" t="n">
         <v>-6675.25</v>
@@ -41752,22 +41737,22 @@
         <v>36182</v>
       </c>
       <c r="H122" t="n">
-        <v>3159.875</v>
+        <v>2558</v>
       </c>
       <c r="I122" t="n">
-        <v>3327</v>
+        <v>2700</v>
       </c>
       <c r="J122" t="n">
         <v>1990</v>
       </c>
       <c r="K122" t="n">
-        <v>9981</v>
+        <v>8100</v>
       </c>
       <c r="L122" t="n">
         <v>5970</v>
       </c>
       <c r="M122" t="n">
-        <v>-7531</v>
+        <v>-5650</v>
       </c>
       <c r="N122" t="n">
         <v>-10870</v>
@@ -41951,25 +41936,25 @@
         <v>36184</v>
       </c>
       <c r="H126" t="n">
-        <v>4525.294</v>
+        <v>5185.6924</v>
       </c>
       <c r="I126" t="n">
-        <v>5343</v>
+        <v>5618.1113</v>
       </c>
       <c r="J126" t="n">
-        <v>3357.1428</v>
+        <v>4212.75</v>
       </c>
       <c r="K126" t="n">
-        <v>16029</v>
+        <v>16854.3339</v>
       </c>
       <c r="L126" t="n">
-        <v>10071.4284</v>
+        <v>12638.25</v>
       </c>
       <c r="M126" t="n">
-        <v>-13559</v>
+        <v>-14384.3339</v>
       </c>
       <c r="N126" t="n">
-        <v>-15011.4284</v>
+        <v>-17578.25</v>
       </c>
     </row>
     <row r="127">
@@ -43028,22 +43013,22 @@
         <v>19744</v>
       </c>
       <c r="H6" t="n">
-        <v>52869.668</v>
+        <v>59150</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>52869.668</v>
+        <v>59150</v>
       </c>
       <c r="K6" t="n">
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>52869.668</v>
+        <v>59150</v>
       </c>
       <c r="N6" t="n">
-        <v>-53093.668</v>
+        <v>-59374</v>
       </c>
     </row>
     <row r="7">
@@ -43328,25 +43313,22 @@
         <v>2654</v>
       </c>
       <c r="H12" t="n">
-        <v>5505.7144</v>
+        <v>899.5</v>
       </c>
       <c r="I12" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>5590</v>
+        <v>899.5</v>
       </c>
       <c r="K12" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>5590</v>
-      </c>
-      <c r="M12" t="n">
-        <v>-4830</v>
+        <v>899.5</v>
       </c>
       <c r="N12" t="n">
-        <v>-5930</v>
+        <v>-1239.5</v>
       </c>
     </row>
     <row r="13">
@@ -43781,25 +43763,25 @@
         <v>2672</v>
       </c>
       <c r="H21" t="n">
-        <v>9001.5</v>
+        <v>7600.2</v>
       </c>
       <c r="I21" t="n">
         <v>30006</v>
       </c>
       <c r="J21" t="n">
-        <v>2000</v>
+        <v>1998.75</v>
       </c>
       <c r="K21" t="n">
         <v>30006</v>
       </c>
       <c r="L21" t="n">
-        <v>2000</v>
+        <v>1998.75</v>
       </c>
       <c r="M21" t="n">
         <v>-29832</v>
       </c>
       <c r="N21" t="n">
-        <v>-2348</v>
+        <v>-2346.75</v>
       </c>
     </row>
     <row r="22">
@@ -43833,25 +43815,25 @@
         <v>5277</v>
       </c>
       <c r="H22" t="n">
-        <v>1724.25</v>
+        <v>1577.4</v>
       </c>
       <c r="I22" t="n">
         <v>1500</v>
       </c>
       <c r="J22" t="n">
-        <v>1948.5</v>
+        <v>1629</v>
       </c>
       <c r="K22" t="n">
         <v>1500</v>
       </c>
       <c r="L22" t="n">
-        <v>1948.5</v>
+        <v>1629</v>
       </c>
       <c r="M22" t="n">
         <v>-1205</v>
       </c>
       <c r="N22" t="n">
-        <v>-2538.5</v>
+        <v>-2219</v>
       </c>
     </row>
     <row r="23">
@@ -44078,25 +44060,25 @@
         <v>5277</v>
       </c>
       <c r="H27" t="n">
-        <v>1724.25</v>
+        <v>1577.4</v>
       </c>
       <c r="I27" t="n">
         <v>1500</v>
       </c>
       <c r="J27" t="n">
-        <v>1948.5</v>
+        <v>1629</v>
       </c>
       <c r="K27" t="n">
         <v>1500</v>
       </c>
       <c r="L27" t="n">
-        <v>1948.5</v>
+        <v>1629</v>
       </c>
       <c r="M27" t="n">
         <v>-1393</v>
       </c>
       <c r="N27" t="n">
-        <v>-2162.5</v>
+        <v>-1843</v>
       </c>
     </row>
     <row r="28">
@@ -44718,22 +44700,22 @@
         <v>36248</v>
       </c>
       <c r="H40" t="n">
-        <v>7583085.5</v>
+        <v>6951592</v>
       </c>
       <c r="I40" t="n">
-        <v>8553378</v>
+        <v>7758196</v>
       </c>
       <c r="J40" t="n">
         <v>14800</v>
       </c>
       <c r="K40" t="n">
-        <v>8553378</v>
+        <v>7758196</v>
       </c>
       <c r="L40" t="n">
         <v>14800</v>
       </c>
       <c r="M40" t="n">
-        <v>-8553242</v>
+        <v>-7758060</v>
       </c>
       <c r="N40" t="n">
         <v>-15072</v>
@@ -45768,25 +45750,25 @@
         <v>27740</v>
       </c>
       <c r="H61" t="n">
-        <v>7011.909</v>
+        <v>5987.3076</v>
       </c>
       <c r="I61" t="n">
-        <v>6869.619</v>
+        <v>6302.6523</v>
       </c>
       <c r="J61" t="n">
-        <v>10000</v>
+        <v>3569.6667</v>
       </c>
       <c r="K61" t="n">
-        <v>6869.619</v>
+        <v>6302.6523</v>
       </c>
       <c r="L61" t="n">
-        <v>10000</v>
+        <v>3569.6667</v>
       </c>
       <c r="M61" t="n">
-        <v>-6667.619</v>
+        <v>-6100.6523</v>
       </c>
       <c r="N61" t="n">
-        <v>-10404</v>
+        <v>-3973.6667</v>
       </c>
     </row>
     <row r="62">
@@ -47351,22 +47333,22 @@
         <v>19993</v>
       </c>
       <c r="H93" t="n">
-        <v>1866.0667</v>
+        <v>1805.6875</v>
       </c>
       <c r="I93" t="n">
-        <v>1450.4</v>
+        <v>1400.3636</v>
       </c>
       <c r="J93" t="n">
         <v>2697.4</v>
       </c>
       <c r="K93" t="n">
-        <v>1450.4</v>
+        <v>1400.3636</v>
       </c>
       <c r="L93" t="n">
         <v>2697.4</v>
       </c>
       <c r="M93" t="n">
-        <v>-202.4000000000001</v>
+        <v>-152.3635999999999</v>
       </c>
       <c r="N93" t="n">
         <v>-5193.4</v>
@@ -48193,22 +48175,22 @@
         <v>25809</v>
       </c>
       <c r="H110" t="n">
-        <v>83214.664</v>
+        <v>79317.75</v>
       </c>
       <c r="I110" t="n">
         <v>0</v>
       </c>
       <c r="J110" t="n">
-        <v>83214.664</v>
+        <v>79317.75</v>
       </c>
       <c r="K110" t="n">
         <v>0</v>
       </c>
       <c r="L110" t="n">
-        <v>83214.664</v>
+        <v>79317.75</v>
       </c>
       <c r="N110" t="n">
-        <v>-91394.664</v>
+        <v>-87497.75</v>
       </c>
     </row>
     <row r="111">
@@ -48340,25 +48322,25 @@
         <v>27740</v>
       </c>
       <c r="H113" t="n">
-        <v>7011.909</v>
+        <v>5987.3076</v>
       </c>
       <c r="I113" t="n">
-        <v>6869.619</v>
+        <v>6302.6523</v>
       </c>
       <c r="J113" t="n">
-        <v>10000</v>
+        <v>3569.6667</v>
       </c>
       <c r="K113" t="n">
-        <v>6869.619</v>
+        <v>6302.6523</v>
       </c>
       <c r="L113" t="n">
-        <v>10000</v>
+        <v>3569.6667</v>
       </c>
       <c r="M113" t="n">
-        <v>-4699.619</v>
+        <v>-4132.6523</v>
       </c>
       <c r="N113" t="n">
-        <v>-14340</v>
+        <v>-7909.6667</v>
       </c>
     </row>
     <row r="114">
@@ -48781,22 +48763,25 @@
         <v>36247</v>
       </c>
       <c r="H122" t="n">
-        <v>5500</v>
+        <v>5198.85</v>
       </c>
       <c r="I122" t="n">
-        <v>0</v>
+        <v>3995.6667</v>
       </c>
       <c r="J122" t="n">
-        <v>5500</v>
+        <v>5411.1763</v>
       </c>
       <c r="K122" t="n">
-        <v>0</v>
+        <v>11987.0001</v>
       </c>
       <c r="L122" t="n">
-        <v>16500</v>
+        <v>16233.5289</v>
+      </c>
+      <c r="M122" t="n">
+        <v>-9537.000100000001</v>
       </c>
       <c r="N122" t="n">
-        <v>-21400</v>
+        <v>-21133.5289</v>
       </c>
     </row>
     <row r="123">
@@ -49855,25 +49840,25 @@
         <v>3307</v>
       </c>
       <c r="H2" t="n">
-        <v>24999.834</v>
+        <v>20499.666</v>
       </c>
       <c r="I2" t="n">
         <v>24499.5</v>
       </c>
       <c r="J2" t="n">
-        <v>25250</v>
+        <v>18499.75</v>
       </c>
       <c r="K2" t="n">
         <v>24499.5</v>
       </c>
       <c r="L2" t="n">
-        <v>25250</v>
+        <v>18499.75</v>
       </c>
       <c r="M2" t="n">
         <v>-24387.5</v>
       </c>
       <c r="N2" t="n">
-        <v>-25474</v>
+        <v>-18723.75</v>
       </c>
     </row>
     <row r="3">
@@ -52852,22 +52837,22 @@
         <v>12589</v>
       </c>
       <c r="H62" t="n">
-        <v>6166.5</v>
+        <v>5833.1665</v>
       </c>
       <c r="I62" t="n">
-        <v>6499</v>
+        <v>4499</v>
       </c>
       <c r="J62" t="n">
         <v>6100</v>
       </c>
       <c r="K62" t="n">
-        <v>6499</v>
+        <v>4499</v>
       </c>
       <c r="L62" t="n">
         <v>6100</v>
       </c>
       <c r="M62" t="n">
-        <v>-5875</v>
+        <v>-3875</v>
       </c>
       <c r="N62" t="n">
         <v>-7348</v>
@@ -52999,22 +52984,22 @@
         <v>12589</v>
       </c>
       <c r="H65" t="n">
-        <v>6166.5</v>
+        <v>5833.1665</v>
       </c>
       <c r="I65" t="n">
-        <v>6499</v>
+        <v>4499</v>
       </c>
       <c r="J65" t="n">
         <v>6100</v>
       </c>
       <c r="K65" t="n">
-        <v>32495</v>
+        <v>22495</v>
       </c>
       <c r="L65" t="n">
         <v>30500</v>
       </c>
       <c r="M65" t="n">
-        <v>-29375</v>
+        <v>-19375</v>
       </c>
       <c r="N65" t="n">
         <v>-36740</v>
@@ -53780,22 +53765,22 @@
         <v>12596</v>
       </c>
       <c r="H81" t="n">
-        <v>203300.2</v>
+        <v>146071.42</v>
       </c>
       <c r="I81" t="n">
-        <v>203300.2</v>
+        <v>146071.42</v>
       </c>
       <c r="J81" t="n">
         <v>0</v>
       </c>
       <c r="K81" t="n">
-        <v>406600.4</v>
+        <v>292142.84</v>
       </c>
       <c r="L81" t="n">
         <v>0</v>
       </c>
       <c r="M81" t="n">
-        <v>-405539.4</v>
+        <v>-291081.84</v>
       </c>
     </row>
     <row r="82">
@@ -53927,22 +53912,22 @@
         <v>12596</v>
       </c>
       <c r="H84" t="n">
-        <v>203300.2</v>
+        <v>146071.42</v>
       </c>
       <c r="I84" t="n">
-        <v>203300.2</v>
+        <v>146071.42</v>
       </c>
       <c r="J84" t="n">
         <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>2033002</v>
+        <v>1460714.2</v>
       </c>
       <c r="L84" t="n">
         <v>0</v>
       </c>
       <c r="M84" t="n">
-        <v>-2027698</v>
+        <v>-1455410.2</v>
       </c>
     </row>
     <row r="85">
@@ -55048,25 +55033,25 @@
         <v>27746</v>
       </c>
       <c r="H107" t="n">
-        <v>560.2727</v>
+        <v>549.64703</v>
       </c>
       <c r="I107" t="n">
         <v>536.76</v>
       </c>
       <c r="J107" t="n">
-        <v>633.75</v>
+        <v>585.44446</v>
       </c>
       <c r="K107" t="n">
         <v>1610.28</v>
       </c>
       <c r="L107" t="n">
-        <v>1901.25</v>
+        <v>1756.33338</v>
       </c>
       <c r="M107" t="n">
         <v>309.72</v>
       </c>
       <c r="N107" t="n">
-        <v>-5741.25</v>
+        <v>-5596.33338</v>
       </c>
     </row>
     <row r="108">
@@ -55391,22 +55376,22 @@
         <v>25978</v>
       </c>
       <c r="H114" t="n">
-        <v>57495</v>
+        <v>55744.75</v>
       </c>
       <c r="I114" t="n">
         <v>0</v>
       </c>
       <c r="J114" t="n">
-        <v>57495</v>
+        <v>55744.75</v>
       </c>
       <c r="K114" t="n">
         <v>0</v>
       </c>
       <c r="L114" t="n">
-        <v>57495</v>
+        <v>55744.75</v>
       </c>
       <c r="N114" t="n">
-        <v>-66173</v>
+        <v>-64422.75</v>
       </c>
     </row>
     <row r="115">
@@ -55835,19 +55820,22 @@
         <v>34127</v>
       </c>
       <c r="H123" t="n">
-        <v>0</v>
+        <v>88000</v>
       </c>
       <c r="I123" t="n">
         <v>0</v>
       </c>
       <c r="J123" t="n">
-        <v>0</v>
+        <v>88000</v>
       </c>
       <c r="K123" t="n">
         <v>0</v>
       </c>
       <c r="L123" t="n">
-        <v>0</v>
+        <v>88000</v>
+      </c>
+      <c r="N123" t="n">
+        <v>-97800</v>
       </c>
     </row>
     <row r="124">
@@ -55979,22 +55967,22 @@
         <v>36210</v>
       </c>
       <c r="H126" t="n">
-        <v>8347.263000000001</v>
+        <v>8728.556</v>
       </c>
       <c r="I126" t="n">
-        <v>7766.3</v>
+        <v>8464.333000000001</v>
       </c>
       <c r="J126" t="n">
         <v>8992.777</v>
       </c>
       <c r="K126" t="n">
-        <v>23298.9</v>
+        <v>25392.999</v>
       </c>
       <c r="L126" t="n">
         <v>26978.331</v>
       </c>
       <c r="M126" t="n">
-        <v>-20828.9</v>
+        <v>-22922.999</v>
       </c>
       <c r="N126" t="n">
         <v>-31918.331</v>
@@ -56273,22 +56261,22 @@
         <v>44029</v>
       </c>
       <c r="H132" t="n">
-        <v>30366.635</v>
+        <v>29147.35</v>
       </c>
       <c r="I132" t="n">
-        <v>46520.043</v>
+        <v>43260.96</v>
       </c>
       <c r="J132" t="n">
         <v>7561.8237</v>
       </c>
       <c r="K132" t="n">
-        <v>139560.129</v>
+        <v>129782.88</v>
       </c>
       <c r="L132" t="n">
         <v>22685.4711</v>
       </c>
       <c r="M132" t="n">
-        <v>-137030.129</v>
+        <v>-127252.88</v>
       </c>
       <c r="N132" t="n">
         <v>-27745.4711</v>

</xml_diff>